<commit_message>
Added data validation lesson in Eglish.
</commit_message>
<xml_diff>
--- a/assets/2022/data-validation/01-data-validation-example-de.xlsx
+++ b/assets/2022/data-validation/01-data-validation-example-de.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{3BCE3B9E-0B79-40D8-AE0C-7FE4A27727E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F746A674-A710-498B-A693-9D44BBF67DE3}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{3BCE3B9E-0B79-40D8-AE0C-7FE4A27727E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8B44714-0F2E-4EC4-ACD1-20485F478426}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{134E06D7-214F-4329-8E1A-B947DBBED7E7}"/>
   </bookViews>
@@ -174,18 +174,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,7 +202,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,18 +498,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1708A1-B03B-4235-80AC-F347E806B164}">
-  <dimension ref="B1:D44"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="4" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" hidden="1"/>
+    <col min="4" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25"/>
@@ -544,90 +545,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="2">
+    <row r="28" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
         <v>12345</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="1" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="1" t="s">
+    <row r="32" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="1" t="s">
+    <row r="36" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="1" t="s">
+    <row r="40" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations xWindow="432" yWindow="691" count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{8F9D3DE9-BCFA-4062-8425-F1C05008F7A5}">
@@ -636,29 +647,29 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{1552013C-5033-4B6B-B2E4-C1003211F95A}">
       <formula1>$B$8:$B$10</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14" xr:uid="{5489E8DA-6CE0-4FDE-A8E5-0339D9171A33}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17" xr:uid="{5489E8DA-6CE0-4FDE-A8E5-0339D9171A33}">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18" xr:uid="{22EE7D32-914D-4536-82C9-A7C18730B1C5}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21" xr:uid="{22EE7D32-914D-4536-82C9-A7C18730B1C5}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hinweis" prompt="Nur ganze Zahlen zwischen 0 und 20 eintragen." sqref="D22" xr:uid="{9F3918C2-C7FC-47CB-A41F-F6B4C83865D0}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hinweis" prompt="Nur ganze Zahlen zwischen 0 und 20 eintragen." sqref="D25" xr:uid="{9F3918C2-C7FC-47CB-A41F-F6B4C83865D0}">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Wert-Quelle" prompt="Geliefert von Max Mustermann am 12/2/2022." sqref="D26" xr:uid="{93EB769A-7EA5-4090-9FF4-D8F6D5D23ADD}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Achtung Achtung!" error="Du hast einen ungültigen Wert eingertragen, das kann ich nicht erlauben." promptTitle="Personalisierte Fehlermeldung" prompt="Einen beliebiegen Wert eintragen, um die Fehlermeldung zu zeigen." sqref="D30" xr:uid="{E83212F1-0025-4B31-9197-DD2A0C36B61B}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Wert-Quelle" prompt="Geliefert von Max Mustermann am 12/2/2022." sqref="D29" xr:uid="{93EB769A-7EA5-4090-9FF4-D8F6D5D23ADD}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Achtung Achtung!" error="Du hast einen ungültigen Wert eingertragen, das kann ich nicht erlauben." promptTitle="Personalisierte Fehlermeldung" prompt="Einen beliebiegen Wert eintragen, um die Fehlermeldung zu zeigen." sqref="D33" xr:uid="{E83212F1-0025-4B31-9197-DD2A0C36B61B}">
       <formula1>FALSE</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pass auf!" error="Du hast einen ungültigen Wert eingertragen. Wenn das genau ist was du willst, dann klicke bitte &quot;Ja&quot;." promptTitle="Warnung-Fehlermeldung" prompt="Einen beliebiegen Wert eintragen, um die Fehlermeldung zu zeigen._x000a_Man kann trotzdem den Wert mit &quot;Ja&quot; eintragen." sqref="D34" xr:uid="{02F1DE90-02B3-4CE6-9D11-FF41E09EB5CD}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pass auf!" error="Du hast einen ungültigen Wert eingertragen. Wenn das genau ist was du willst, dann klicke bitte &quot;Ja&quot;." promptTitle="Warnung-Fehlermeldung" prompt="Einen beliebiegen Wert eintragen, um die Fehlermeldung zu zeigen._x000a_Man kann trotzdem den Wert mit &quot;Ja&quot; eintragen." sqref="D37" xr:uid="{02F1DE90-02B3-4CE6-9D11-FF41E09EB5CD}">
       <formula1>FALSE</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Oh nein!" error="Du hast einen nicht vorgesehen Wert eingertragen, ich werde dich aber nicht halten." promptTitle="Information-Fehlermeldung" prompt="Einen beliebiegen Wert eintragen, um die Fehlermeldung zu zeigen._x000a_Jeder Wert wird akzeptiert, solange man &quot;OK&quot; klickt." sqref="D38" xr:uid="{6D712824-F542-4484-86ED-F8D824D94388}">
+    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Oh nein!" error="Du hast einen nicht vorgesehen Wert eingertragen, ich werde dich aber nicht halten." promptTitle="Information-Fehlermeldung" prompt="Einen beliebiegen Wert eintragen, um die Fehlermeldung zu zeigen._x000a_Jeder Wert wird akzeptiert, solange man &quot;OK&quot; klickt." sqref="D41" xr:uid="{6D712824-F542-4484-86ED-F8D824D94388}">
       <formula1>FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Fehlermeldung deaktiviert" prompt="Hier kann man eine Option aus dem Dropdown auswählen oder einen personalisierten Wert eintragen." sqref="D42" xr:uid="{35C97A75-CF6A-4036-9191-BF1C6C8F1BBA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Fehlermeldung deaktiviert" prompt="Hier kann man eine Option aus dem Dropdown auswählen oder einen personalisierten Wert eintragen." sqref="D45" xr:uid="{35C97A75-CF6A-4036-9191-BF1C6C8F1BBA}">
       <formula1>"Apfel, Banane, Orange"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>